<commit_message>
flicking version, trying new way to draw it
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -342,10 +342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB22"/>
+  <dimension ref="A1:AJ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AA19" sqref="AA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -373,9 +373,15 @@
     <col min="25" max="26" width="3.28515625" customWidth="1"/>
     <col min="27" max="27" width="2.85546875" customWidth="1"/>
     <col min="28" max="28" width="3.140625" customWidth="1"/>
+    <col min="29" max="31" width="3" customWidth="1"/>
+    <col min="32" max="32" width="2.7109375" customWidth="1"/>
+    <col min="33" max="33" width="2.5703125" customWidth="1"/>
+    <col min="34" max="34" width="2.7109375" customWidth="1"/>
+    <col min="35" max="35" width="3" customWidth="1"/>
+    <col min="36" max="36" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:36">
       <c r="A1">
         <v>1</v>
       </c>
@@ -460,129 +466,177 @@
       <c r="AB1">
         <v>1</v>
       </c>
+      <c r="AC1">
+        <v>1</v>
+      </c>
+      <c r="AD1">
+        <v>1</v>
+      </c>
+      <c r="AE1">
+        <v>1</v>
+      </c>
+      <c r="AF1">
+        <v>1</v>
+      </c>
+      <c r="AG1">
+        <v>1</v>
+      </c>
+      <c r="AH1">
+        <v>1</v>
+      </c>
+      <c r="AI1">
+        <v>1</v>
+      </c>
+      <c r="AJ1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:36">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB2">
         <v>1</v>
       </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AG2">
+        <v>1</v>
+      </c>
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AI2">
+        <v>1</v>
+      </c>
+      <c r="AJ2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:36">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -594,167 +648,215 @@
         <v>1</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB3">
         <v>1</v>
       </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:36">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB4">
         <v>1</v>
       </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4">
+        <v>1</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4">
+        <v>1</v>
+      </c>
+      <c r="AH4">
+        <v>1</v>
+      </c>
+      <c r="AI4">
+        <v>1</v>
+      </c>
+      <c r="AJ4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:36">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -766,63 +868,87 @@
         <v>1</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB5">
         <v>1</v>
       </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:36">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -834,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -843,25 +969,25 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -870,7 +996,7 @@
         <v>0</v>
       </c>
       <c r="V6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -888,27 +1014,51 @@
         <v>0</v>
       </c>
       <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>1</v>
+      </c>
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AI6">
+        <v>1</v>
+      </c>
+      <c r="AJ6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:36">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -920,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -929,25 +1079,25 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -956,7 +1106,7 @@
         <v>0</v>
       </c>
       <c r="V7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -974,39 +1124,63 @@
         <v>0</v>
       </c>
       <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
+        <v>1</v>
+      </c>
+      <c r="AI7">
+        <v>1</v>
+      </c>
+      <c r="AJ7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:36">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1015,28 +1189,28 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S8">
         <v>2</v>
       </c>
       <c r="T8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -1045,7 +1219,7 @@
         <v>2</v>
       </c>
       <c r="W8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -1060,39 +1234,63 @@
         <v>0</v>
       </c>
       <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+      <c r="AG8">
+        <v>1</v>
+      </c>
+      <c r="AH8">
+        <v>1</v>
+      </c>
+      <c r="AI8">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:36">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>2</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1101,28 +1299,28 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -1131,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="W9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X9">
         <v>0</v>
@@ -1140,45 +1338,69 @@
         <v>0</v>
       </c>
       <c r="Z9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB9">
+        <v>2</v>
+      </c>
+      <c r="AC9">
+        <v>2</v>
+      </c>
+      <c r="AD9">
+        <v>2</v>
+      </c>
+      <c r="AE9">
+        <v>2</v>
+      </c>
+      <c r="AF9">
+        <v>1</v>
+      </c>
+      <c r="AG9">
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AI9">
+        <v>1</v>
+      </c>
+      <c r="AJ9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:36">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1190,7 +1412,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1199,16 +1421,16 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -1226,45 +1448,69 @@
         <v>0</v>
       </c>
       <c r="Z10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA10">
         <v>0</v>
       </c>
       <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>1</v>
+      </c>
+      <c r="AG10">
+        <v>1</v>
+      </c>
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:36">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1276,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -1285,22 +1531,22 @@
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W11">
         <v>0</v>
@@ -1312,30 +1558,54 @@
         <v>0</v>
       </c>
       <c r="Z11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA11">
         <v>0</v>
       </c>
       <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>1</v>
+      </c>
+      <c r="AG11">
+        <v>1</v>
+      </c>
+      <c r="AH11">
+        <v>1</v>
+      </c>
+      <c r="AI11">
+        <v>1</v>
+      </c>
+      <c r="AJ11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:36">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1350,19 +1620,19 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -1371,13 +1641,13 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T12">
         <v>0</v>
@@ -1386,42 +1656,66 @@
         <v>0</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y12">
         <v>0</v>
       </c>
       <c r="Z12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>1</v>
+      </c>
+      <c r="AG12">
+        <v>1</v>
+      </c>
+      <c r="AH12">
+        <v>1</v>
+      </c>
+      <c r="AI12">
+        <v>1</v>
+      </c>
+      <c r="AJ12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:36">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1433,16 +1727,16 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1457,13 +1751,13 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T13">
         <v>0</v>
@@ -1478,36 +1772,60 @@
         <v>0</v>
       </c>
       <c r="X13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y13">
         <v>0</v>
       </c>
       <c r="Z13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>1</v>
+      </c>
+      <c r="AG13">
+        <v>1</v>
+      </c>
+      <c r="AH13">
+        <v>1</v>
+      </c>
+      <c r="AI13">
+        <v>1</v>
+      </c>
+      <c r="AJ13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:36">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1519,16 +1837,16 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1564,36 +1882,60 @@
         <v>0</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y14">
         <v>0</v>
       </c>
       <c r="Z14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA14">
         <v>0</v>
       </c>
       <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>1</v>
+      </c>
+      <c r="AG14">
+        <v>1</v>
+      </c>
+      <c r="AH14">
+        <v>1</v>
+      </c>
+      <c r="AI14">
+        <v>1</v>
+      </c>
+      <c r="AJ14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:36">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1608,13 +1950,13 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1650,36 +1992,60 @@
         <v>0</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA15">
         <v>0</v>
       </c>
       <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>1</v>
+      </c>
+      <c r="AG15">
+        <v>1</v>
+      </c>
+      <c r="AH15">
+        <v>1</v>
+      </c>
+      <c r="AI15">
+        <v>1</v>
+      </c>
+      <c r="AJ15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:36">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1691,37 +2057,37 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T16">
         <v>0</v>
@@ -1748,24 +2114,48 @@
         <v>0</v>
       </c>
       <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>1</v>
+      </c>
+      <c r="AG16">
+        <v>1</v>
+      </c>
+      <c r="AH16">
+        <v>1</v>
+      </c>
+      <c r="AI16">
+        <v>1</v>
+      </c>
+      <c r="AJ16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:36">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1798,19 +2188,19 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -1834,24 +2224,48 @@
         <v>0</v>
       </c>
       <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>1</v>
+      </c>
+      <c r="AG17">
+        <v>1</v>
+      </c>
+      <c r="AH17">
+        <v>1</v>
+      </c>
+      <c r="AI17">
+        <v>1</v>
+      </c>
+      <c r="AJ17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:36">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1920,24 +2334,48 @@
         <v>0</v>
       </c>
       <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>1</v>
+      </c>
+      <c r="AG18">
+        <v>1</v>
+      </c>
+      <c r="AH18">
+        <v>1</v>
+      </c>
+      <c r="AI18">
+        <v>1</v>
+      </c>
+      <c r="AJ18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:36">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1949,10 +2387,10 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -2000,30 +2438,54 @@
         <v>0</v>
       </c>
       <c r="Z19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>1</v>
+      </c>
+      <c r="AG19">
+        <v>1</v>
+      </c>
+      <c r="AH19">
+        <v>1</v>
+      </c>
+      <c r="AI19">
+        <v>1</v>
+      </c>
+      <c r="AJ19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:36">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -2038,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -2047,37 +2509,37 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X20">
         <v>0</v>
@@ -2086,30 +2548,54 @@
         <v>0</v>
       </c>
       <c r="Z20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA20">
         <v>0</v>
       </c>
       <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>1</v>
+      </c>
+      <c r="AG20">
+        <v>1</v>
+      </c>
+      <c r="AH20">
+        <v>1</v>
+      </c>
+      <c r="AI20">
+        <v>1</v>
+      </c>
+      <c r="AJ20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:36">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -2124,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -2172,16 +2658,40 @@
         <v>0</v>
       </c>
       <c r="Z21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA21">
         <v>0</v>
       </c>
       <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>1</v>
+      </c>
+      <c r="AG21">
+        <v>1</v>
+      </c>
+      <c r="AH21">
+        <v>1</v>
+      </c>
+      <c r="AI21">
+        <v>1</v>
+      </c>
+      <c r="AJ21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:36">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2198,77 +2708,982 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>1</v>
+      </c>
+      <c r="AG22">
+        <v>1</v>
+      </c>
+      <c r="AH22">
+        <v>1</v>
+      </c>
+      <c r="AI22">
+        <v>1</v>
+      </c>
+      <c r="AJ22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>1</v>
+      </c>
+      <c r="AG23">
+        <v>1</v>
+      </c>
+      <c r="AH23">
+        <v>1</v>
+      </c>
+      <c r="AI23">
+        <v>1</v>
+      </c>
+      <c r="AJ23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <v>1</v>
+      </c>
+      <c r="AG24">
+        <v>1</v>
+      </c>
+      <c r="AH24">
+        <v>1</v>
+      </c>
+      <c r="AI24">
+        <v>1</v>
+      </c>
+      <c r="AJ24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <v>1</v>
+      </c>
+      <c r="AG25">
+        <v>1</v>
+      </c>
+      <c r="AH25">
+        <v>1</v>
+      </c>
+      <c r="AI25">
+        <v>1</v>
+      </c>
+      <c r="AJ25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26">
+        <v>1</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26">
+        <v>1</v>
+      </c>
+      <c r="Y26">
+        <v>1</v>
+      </c>
+      <c r="Z26">
+        <v>1</v>
+      </c>
+      <c r="AA26">
+        <v>1</v>
+      </c>
+      <c r="AB26">
+        <v>1</v>
+      </c>
+      <c r="AC26">
+        <v>1</v>
+      </c>
+      <c r="AD26">
+        <v>1</v>
+      </c>
+      <c r="AE26">
+        <v>1</v>
+      </c>
+      <c r="AF26">
+        <v>1</v>
+      </c>
+      <c r="AG26">
+        <v>1</v>
+      </c>
+      <c r="AH26">
+        <v>1</v>
+      </c>
+      <c r="AI26">
+        <v>1</v>
+      </c>
+      <c r="AJ26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="X27">
+        <v>1</v>
+      </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="Z27">
+        <v>1</v>
+      </c>
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AB27">
+        <v>1</v>
+      </c>
+      <c r="AC27">
+        <v>1</v>
+      </c>
+      <c r="AD27">
+        <v>1</v>
+      </c>
+      <c r="AE27">
+        <v>1</v>
+      </c>
+      <c r="AF27">
+        <v>1</v>
+      </c>
+      <c r="AG27">
+        <v>1</v>
+      </c>
+      <c r="AH27">
+        <v>1</v>
+      </c>
+      <c r="AI27">
+        <v>1</v>
+      </c>
+      <c r="AJ27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
+      <c r="U28">
+        <v>1</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>1</v>
+      </c>
+      <c r="X28">
+        <v>1</v>
+      </c>
+      <c r="Y28">
+        <v>1</v>
+      </c>
+      <c r="Z28">
+        <v>1</v>
+      </c>
+      <c r="AA28">
+        <v>1</v>
+      </c>
+      <c r="AB28">
+        <v>1</v>
+      </c>
+      <c r="AC28">
+        <v>1</v>
+      </c>
+      <c r="AD28">
+        <v>1</v>
+      </c>
+      <c r="AE28">
+        <v>1</v>
+      </c>
+      <c r="AF28">
+        <v>1</v>
+      </c>
+      <c r="AG28">
+        <v>1</v>
+      </c>
+      <c r="AH28">
+        <v>1</v>
+      </c>
+      <c r="AI28">
+        <v>1</v>
+      </c>
+      <c r="AJ28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <v>1</v>
+      </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29">
+        <v>1</v>
+      </c>
+      <c r="Y29">
+        <v>1</v>
+      </c>
+      <c r="Z29">
+        <v>1</v>
+      </c>
+      <c r="AA29">
+        <v>1</v>
+      </c>
+      <c r="AB29">
+        <v>1</v>
+      </c>
+      <c r="AC29">
+        <v>1</v>
+      </c>
+      <c r="AD29">
+        <v>1</v>
+      </c>
+      <c r="AE29">
+        <v>1</v>
+      </c>
+      <c r="AF29">
+        <v>1</v>
+      </c>
+      <c r="AG29">
+        <v>1</v>
+      </c>
+      <c r="AH29">
+        <v>1</v>
+      </c>
+      <c r="AI29">
+        <v>1</v>
+      </c>
+      <c r="AJ29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="V30">
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>1</v>
+      </c>
+      <c r="Y30">
+        <v>1</v>
+      </c>
+      <c r="Z30">
+        <v>1</v>
+      </c>
+      <c r="AA30">
+        <v>1</v>
+      </c>
+      <c r="AB30">
+        <v>1</v>
+      </c>
+      <c r="AC30">
+        <v>1</v>
+      </c>
+      <c r="AD30">
+        <v>1</v>
+      </c>
+      <c r="AE30">
+        <v>1</v>
+      </c>
+      <c r="AF30">
+        <v>1</v>
+      </c>
+      <c r="AG30">
+        <v>1</v>
+      </c>
+      <c r="AH30">
+        <v>1</v>
+      </c>
+      <c r="AI30">
+        <v>1</v>
+      </c>
+      <c r="AJ30">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Tank and bullet collision, big explosion handled
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -342,10 +342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ30"/>
+  <dimension ref="A1:AL37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AA19" sqref="AA19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="AP17" sqref="AP17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -379,573 +379,605 @@
     <col min="34" max="34" width="2.7109375" customWidth="1"/>
     <col min="35" max="35" width="3" customWidth="1"/>
     <col min="36" max="36" width="3.140625" customWidth="1"/>
+    <col min="37" max="37" width="3.5703125" customWidth="1"/>
+    <col min="38" max="38" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:38">
       <c r="A1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK1">
+        <v>0</v>
+      </c>
+      <c r="AL1">
+        <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:38">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:38">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:38">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:38">
       <c r="A5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5">
         <v>1</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <v>1</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ5">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:38">
       <c r="A6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -981,13 +1013,13 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -1026,36 +1058,42 @@
         <v>0</v>
       </c>
       <c r="AF6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ6">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:38">
       <c r="A7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1091,13 +1129,13 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -1136,36 +1174,42 @@
         <v>0</v>
       </c>
       <c r="AF7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ7">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:38">
       <c r="A8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1192,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -1201,13 +1245,13 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -1216,7 +1260,7 @@
         <v>0</v>
       </c>
       <c r="V8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -1246,69 +1290,75 @@
         <v>0</v>
       </c>
       <c r="AF8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ8">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:38">
       <c r="A9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <v>1</v>
@@ -1320,40 +1370,40 @@
         <v>1</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF9">
         <v>1</v>
@@ -1362,33 +1412,39 @@
         <v>1</v>
       </c>
       <c r="AH9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ9">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:38">
       <c r="A10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1400,7 +1456,7 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1412,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1421,22 +1477,22 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -1448,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="Z10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA10">
         <v>0</v>
@@ -1466,39 +1522,45 @@
         <v>0</v>
       </c>
       <c r="AF10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG10">
         <v>1</v>
       </c>
       <c r="AH10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ10">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:38">
       <c r="A11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1510,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1522,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -1531,22 +1593,22 @@
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R11">
         <v>1</v>
       </c>
       <c r="S11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W11">
         <v>0</v>
@@ -1558,7 +1620,7 @@
         <v>0</v>
       </c>
       <c r="Z11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA11">
         <v>0</v>
@@ -1576,39 +1638,45 @@
         <v>0</v>
       </c>
       <c r="AF11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG11">
         <v>1</v>
       </c>
       <c r="AH11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ11">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:38">
       <c r="A12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1620,19 +1688,19 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -1641,37 +1709,37 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y12">
         <v>0</v>
       </c>
       <c r="Z12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB12">
         <v>0</v>
@@ -1686,45 +1754,51 @@
         <v>0</v>
       </c>
       <c r="AF12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG12">
         <v>1</v>
       </c>
       <c r="AH12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ12">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK12">
+        <v>0</v>
+      </c>
+      <c r="AL12">
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:38">
       <c r="A13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -1736,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1751,19 +1825,19 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13">
         <v>1</v>
       </c>
       <c r="S13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -1772,63 +1846,69 @@
         <v>0</v>
       </c>
       <c r="X13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y13">
         <v>0</v>
       </c>
       <c r="Z13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB13">
         <v>0</v>
       </c>
       <c r="AC13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG13">
         <v>1</v>
       </c>
       <c r="AH13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ13">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <v>0</v>
+      </c>
+      <c r="AL13">
+        <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:38">
       <c r="A14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1837,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>2</v>
@@ -1846,7 +1926,7 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1864,16 +1944,16 @@
         <v>0</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <v>0</v>
@@ -1882,13 +1962,13 @@
         <v>0</v>
       </c>
       <c r="X14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y14">
         <v>0</v>
       </c>
       <c r="Z14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA14">
         <v>0</v>
@@ -1897,7 +1977,7 @@
         <v>0</v>
       </c>
       <c r="AC14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -1906,39 +1986,45 @@
         <v>0</v>
       </c>
       <c r="AF14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG14">
         <v>1</v>
       </c>
       <c r="AH14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ14">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:38">
       <c r="A15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1953,10 +2039,10 @@
         <v>2</v>
       </c>
       <c r="K15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1974,16 +2060,16 @@
         <v>0</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -1992,13 +2078,13 @@
         <v>0</v>
       </c>
       <c r="X15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA15">
         <v>0</v>
@@ -2007,7 +2093,7 @@
         <v>0</v>
       </c>
       <c r="AC15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD15">
         <v>0</v>
@@ -2016,39 +2102,45 @@
         <v>0</v>
       </c>
       <c r="AF15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG15">
         <v>1</v>
       </c>
       <c r="AH15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ15">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK15">
+        <v>0</v>
+      </c>
+      <c r="AL15">
+        <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:38">
       <c r="A16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -2060,16 +2152,16 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -2084,16 +2176,16 @@
         <v>0</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V16">
         <v>0</v>
@@ -2108,16 +2200,16 @@
         <v>0</v>
       </c>
       <c r="Z16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB16">
         <v>0</v>
       </c>
       <c r="AC16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD16">
         <v>0</v>
@@ -2126,39 +2218,45 @@
         <v>0</v>
       </c>
       <c r="AF16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG16">
         <v>1</v>
       </c>
       <c r="AH16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ16">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK16">
+        <v>0</v>
+      </c>
+      <c r="AL16">
+        <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:38">
       <c r="A17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -2167,16 +2265,16 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -2188,22 +2286,22 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S17">
         <v>2</v>
       </c>
       <c r="T17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -2221,54 +2319,60 @@
         <v>0</v>
       </c>
       <c r="AA17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB17">
         <v>0</v>
       </c>
       <c r="AC17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE17">
         <v>0</v>
       </c>
       <c r="AF17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG17">
         <v>1</v>
       </c>
       <c r="AH17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ17">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:38">
       <c r="A18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -2277,16 +2381,16 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -2331,54 +2435,60 @@
         <v>0</v>
       </c>
       <c r="AA18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB18">
         <v>0</v>
       </c>
       <c r="AC18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE18">
         <v>0</v>
       </c>
       <c r="AF18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG18">
         <v>1</v>
       </c>
       <c r="AH18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ18">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK18">
+        <v>0</v>
+      </c>
+      <c r="AL18">
+        <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:38">
       <c r="A19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -2387,16 +2497,16 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <v>2</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -2438,16 +2548,16 @@
         <v>0</v>
       </c>
       <c r="Z19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA19">
         <v>2</v>
       </c>
       <c r="AB19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD19">
         <v>0</v>
@@ -2456,39 +2566,45 @@
         <v>0</v>
       </c>
       <c r="AF19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG19">
         <v>1</v>
       </c>
       <c r="AH19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ19">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK19">
+        <v>0</v>
+      </c>
+      <c r="AL19">
+        <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:38">
       <c r="A20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -2500,7 +2616,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -2509,37 +2625,37 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X20">
         <v>0</v>
@@ -2548,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="Z20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA20">
         <v>0</v>
@@ -2566,39 +2682,45 @@
         <v>0</v>
       </c>
       <c r="AF20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG20">
         <v>1</v>
       </c>
       <c r="AH20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ20">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK20">
+        <v>0</v>
+      </c>
+      <c r="AL20">
+        <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:38">
       <c r="A21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2610,7 +2732,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -2634,16 +2756,16 @@
         <v>0</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V21">
         <v>0</v>
@@ -2658,7 +2780,7 @@
         <v>0</v>
       </c>
       <c r="Z21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA21">
         <v>0</v>
@@ -2676,39 +2798,45 @@
         <v>0</v>
       </c>
       <c r="AF21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG21">
         <v>1</v>
       </c>
       <c r="AH21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ21">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK21">
+        <v>0</v>
+      </c>
+      <c r="AL21">
+        <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:36">
+    <row r="22" spans="1:38">
       <c r="A22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2717,10 +2845,10 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -2768,10 +2896,10 @@
         <v>0</v>
       </c>
       <c r="Z22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB22">
         <v>0</v>
@@ -2786,39 +2914,45 @@
         <v>0</v>
       </c>
       <c r="AF22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG22">
         <v>1</v>
       </c>
       <c r="AH22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ22">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK22">
+        <v>0</v>
+      </c>
+      <c r="AL22">
+        <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:36">
+    <row r="23" spans="1:38">
       <c r="A23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -2833,10 +2967,10 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -2881,10 +3015,10 @@
         <v>0</v>
       </c>
       <c r="AA23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC23">
         <v>0</v>
@@ -2896,39 +3030,45 @@
         <v>0</v>
       </c>
       <c r="AF23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG23">
         <v>1</v>
       </c>
       <c r="AH23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ23">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:36">
+    <row r="24" spans="1:38">
       <c r="A24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -2946,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -2958,28 +3098,28 @@
         <v>0</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X24">
         <v>0</v>
@@ -2991,7 +3131,7 @@
         <v>0</v>
       </c>
       <c r="AA24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB24">
         <v>0</v>
@@ -3006,39 +3146,45 @@
         <v>0</v>
       </c>
       <c r="AF24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG24">
         <v>1</v>
       </c>
       <c r="AH24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ24">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK24">
+        <v>0</v>
+      </c>
+      <c r="AL24">
+        <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:36">
+    <row r="25" spans="1:38">
       <c r="A25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -3056,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -3101,7 +3247,7 @@
         <v>0</v>
       </c>
       <c r="AA25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB25">
         <v>0</v>
@@ -3116,476 +3262,506 @@
         <v>0</v>
       </c>
       <c r="AF25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG25">
         <v>1</v>
       </c>
       <c r="AH25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ25">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK25">
+        <v>0</v>
+      </c>
+      <c r="AL25">
+        <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:36">
+    <row r="26" spans="1:38">
       <c r="A26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG26">
         <v>1</v>
       </c>
       <c r="AH26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ26">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK26">
+        <v>0</v>
+      </c>
+      <c r="AL26">
+        <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:36">
+    <row r="27" spans="1:38">
       <c r="A27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG27">
         <v>1</v>
       </c>
       <c r="AH27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ27">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK27">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:36">
+    <row r="28" spans="1:38">
       <c r="A28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG28">
         <v>1</v>
       </c>
       <c r="AH28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ28">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK28">
+        <v>0</v>
+      </c>
+      <c r="AL28">
+        <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:36">
+    <row r="29" spans="1:38">
       <c r="A29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG29">
         <v>1</v>
       </c>
       <c r="AH29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ29">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK29">
+        <v>0</v>
+      </c>
+      <c r="AL29">
+        <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:36">
+    <row r="30" spans="1:38">
       <c r="A30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -3672,13 +3848,831 @@
         <v>1</v>
       </c>
       <c r="AH30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ30">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AK30">
+        <v>0</v>
+      </c>
+      <c r="AL30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>0</v>
+      </c>
+      <c r="AA31">
+        <v>0</v>
+      </c>
+      <c r="AB31">
+        <v>0</v>
+      </c>
+      <c r="AC31">
+        <v>0</v>
+      </c>
+      <c r="AD31">
+        <v>0</v>
+      </c>
+      <c r="AE31">
+        <v>0</v>
+      </c>
+      <c r="AF31">
+        <v>0</v>
+      </c>
+      <c r="AG31">
+        <v>0</v>
+      </c>
+      <c r="AH31">
+        <v>0</v>
+      </c>
+      <c r="AI31">
+        <v>0</v>
+      </c>
+      <c r="AJ31">
+        <v>0</v>
+      </c>
+      <c r="AK31">
+        <v>0</v>
+      </c>
+      <c r="AL31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+      <c r="AB32">
+        <v>0</v>
+      </c>
+      <c r="AC32">
+        <v>0</v>
+      </c>
+      <c r="AD32">
+        <v>0</v>
+      </c>
+      <c r="AE32">
+        <v>0</v>
+      </c>
+      <c r="AF32">
+        <v>0</v>
+      </c>
+      <c r="AG32">
+        <v>0</v>
+      </c>
+      <c r="AH32">
+        <v>0</v>
+      </c>
+      <c r="AI32">
+        <v>0</v>
+      </c>
+      <c r="AJ32">
+        <v>0</v>
+      </c>
+      <c r="AK32">
+        <v>0</v>
+      </c>
+      <c r="AL32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+      <c r="Y33">
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>0</v>
+      </c>
+      <c r="AB33">
+        <v>0</v>
+      </c>
+      <c r="AC33">
+        <v>0</v>
+      </c>
+      <c r="AD33">
+        <v>0</v>
+      </c>
+      <c r="AE33">
+        <v>0</v>
+      </c>
+      <c r="AF33">
+        <v>0</v>
+      </c>
+      <c r="AG33">
+        <v>0</v>
+      </c>
+      <c r="AH33">
+        <v>0</v>
+      </c>
+      <c r="AI33">
+        <v>0</v>
+      </c>
+      <c r="AJ33">
+        <v>0</v>
+      </c>
+      <c r="AK33">
+        <v>0</v>
+      </c>
+      <c r="AL33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <v>0</v>
+      </c>
+      <c r="AB34">
+        <v>0</v>
+      </c>
+      <c r="AC34">
+        <v>0</v>
+      </c>
+      <c r="AD34">
+        <v>0</v>
+      </c>
+      <c r="AE34">
+        <v>0</v>
+      </c>
+      <c r="AF34">
+        <v>0</v>
+      </c>
+      <c r="AG34">
+        <v>0</v>
+      </c>
+      <c r="AH34">
+        <v>0</v>
+      </c>
+      <c r="AI34">
+        <v>0</v>
+      </c>
+      <c r="AJ34">
+        <v>0</v>
+      </c>
+      <c r="AK34">
+        <v>0</v>
+      </c>
+      <c r="AL34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>0</v>
+      </c>
+      <c r="Z35">
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <v>0</v>
+      </c>
+      <c r="AB35">
+        <v>0</v>
+      </c>
+      <c r="AC35">
+        <v>0</v>
+      </c>
+      <c r="AD35">
+        <v>0</v>
+      </c>
+      <c r="AE35">
+        <v>0</v>
+      </c>
+      <c r="AF35">
+        <v>0</v>
+      </c>
+      <c r="AG35">
+        <v>0</v>
+      </c>
+      <c r="AH35">
+        <v>0</v>
+      </c>
+      <c r="AI35">
+        <v>0</v>
+      </c>
+      <c r="AJ35">
+        <v>0</v>
+      </c>
+      <c r="AK35">
+        <v>0</v>
+      </c>
+      <c r="AL35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <v>0</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <v>0</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
+      <c r="AA36">
+        <v>0</v>
+      </c>
+      <c r="AB36">
+        <v>0</v>
+      </c>
+      <c r="AC36">
+        <v>0</v>
+      </c>
+      <c r="AD36">
+        <v>0</v>
+      </c>
+      <c r="AE36">
+        <v>0</v>
+      </c>
+      <c r="AF36">
+        <v>0</v>
+      </c>
+      <c r="AG36">
+        <v>0</v>
+      </c>
+      <c r="AH36">
+        <v>0</v>
+      </c>
+      <c r="AI36">
+        <v>0</v>
+      </c>
+      <c r="AJ36">
+        <v>0</v>
+      </c>
+      <c r="AK36">
+        <v>0</v>
+      </c>
+      <c r="AL36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+      <c r="Y37">
+        <v>0</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37">
+        <v>0</v>
+      </c>
+      <c r="AB37">
+        <v>0</v>
+      </c>
+      <c r="AC37">
+        <v>0</v>
+      </c>
+      <c r="AD37">
+        <v>0</v>
+      </c>
+      <c r="AE37">
+        <v>0</v>
+      </c>
+      <c r="AF37">
+        <v>0</v>
+      </c>
+      <c r="AG37">
+        <v>0</v>
+      </c>
+      <c r="AH37">
+        <v>0</v>
+      </c>
+      <c r="AI37">
+        <v>0</v>
+      </c>
+      <c r="AJ37">
+        <v>0</v>
+      </c>
+      <c r="AK37">
+        <v>0</v>
+      </c>
+      <c r="AL37">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tank collision handled, new map
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -344,8 +344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AL37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2967,7 +2967,7 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L23">
         <v>2</v>
@@ -3018,7 +3018,7 @@
         <v>2</v>
       </c>
       <c r="AB23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC23">
         <v>0</v>
@@ -3086,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -3107,10 +3107,10 @@
         <v>2</v>
       </c>
       <c r="S24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U24">
         <v>2</v>
@@ -3131,7 +3131,7 @@
         <v>0</v>
       </c>
       <c r="AA24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB24">
         <v>0</v>
@@ -3190,7 +3190,7 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -3202,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -3247,7 +3247,7 @@
         <v>0</v>
       </c>
       <c r="AA25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB25">
         <v>0</v>
@@ -3315,7 +3315,7 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L26">
         <v>2</v>
@@ -3366,7 +3366,7 @@
         <v>2</v>
       </c>
       <c r="AB26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC26">
         <v>0</v>
@@ -3553,7 +3553,7 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N28">
         <v>0</v>

</xml_diff>